<commit_message>
updated mappings and pres
</commit_message>
<xml_diff>
--- a/documents/mappings/EDAC-to-OBOE.xlsx
+++ b/documents/mappings/EDAC-to-OBOE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -181,8 +181,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -237,7 +241,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -258,6 +262,8 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -278,6 +284,8 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -610,7 +618,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -657,7 +665,7 @@
         <v>20</v>
       </c>
       <c r="D2" s="4">
-        <v>1530</v>
+        <v>1532</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>9</v>
@@ -678,7 +686,7 @@
         <v>21</v>
       </c>
       <c r="D3" s="4">
-        <v>24</v>
+        <v>1532</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>10</v>
@@ -699,7 +707,7 @@
         <v>20</v>
       </c>
       <c r="D4" s="4">
-        <v>918</v>
+        <v>3064</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>9</v>

</xml_diff>